<commit_message>
Updated Test Case file
</commit_message>
<xml_diff>
--- a/Test_Case.xlsx
+++ b/Test_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manual Testing For HSC Formula Aid App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2522F45-2B57-49CA-AA3D-981707BD2136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0E7852-CB02-476F-B365-33A434EDFE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{690E196A-54C6-4629-9049-4FB181315749}"/>
   </bookViews>
@@ -101,24 +101,7 @@
     <t>App installed on both Android and iPhone</t>
   </si>
   <si>
-    <t>1. Open app on Android device
-2. Access hamburger menu
-3. Note all available options
-4. Open app on iPhone
-5. Access hamburger menu
-6. Compare options between platforms</t>
-  </si>
-  <si>
-    <t>Hamburger menu should have identical options on both Android and iPhone</t>
-  </si>
-  <si>
-    <t>Hamburger menu has same options for Android and iPhone, but 2 options are missing for iPhone while available for Android</t>
-  </si>
-  <si>
     <t>App launched, content accessible</t>
-  </si>
-  <si>
-    <t>Clear text hierarchy with consistent heading styles, proper typography levels</t>
   </si>
   <si>
     <t>App launched, content sections accessible</t>
@@ -142,19 +125,10 @@
     <t>All elements should be properly aligned according to design guidelines</t>
   </si>
   <si>
-    <t>Platform inconsistency:  iPhone missing 2 menu options. Cross-platform inconsistency affecting user experience.</t>
-  </si>
-  <si>
-    <t>Heading styles and text hierarchy need standardization. Affects content readability and user navigation.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Verify proper spacing between UI elements and content sections</t>
   </si>
   <si>
     <t xml:space="preserve"> Verify text hierarchy implementation</t>
-  </si>
-  <si>
-    <t>Test hamburger menu options consistency across platforms</t>
   </si>
   <si>
     <t>Check subjects priority and organization</t>
@@ -350,9 +324,6 @@
 </t>
   </si>
   <si>
-    <t>Example content should load within 3-4 seconds</t>
-  </si>
-  <si>
     <t>Some example loading time is not acceptable</t>
   </si>
   <si>
@@ -376,16 +347,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pages are not full screen and page number shows the half page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Navigate to any subject section
-2. Observe heading styles
-3. Check subheading formatting
-4. Verify body text formatting
-5. Verify consistency across sections                                                                 6. Verify every page has text </t>
-  </si>
-  <si>
-    <t>Text hierarchy implementation is inconsistent across different sections and some pages are blank</t>
   </si>
   <si>
     <t>Page layout is not satisfactory and page number is improper</t>
@@ -571,18 +532,9 @@
 </t>
   </si>
   <si>
-    <t>Verify every chapter has same content</t>
-  </si>
-  <si>
     <t xml:space="preserve">App launched with accessable chapter </t>
   </si>
   <si>
-    <t>Every chapter should same content or section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Physics, there are some chapters have short questions, while others do not </t>
-  </si>
-  <si>
     <t xml:space="preserve">Every chapter needs content completion </t>
   </si>
   <si>
@@ -593,10 +545,6 @@
   </si>
   <si>
     <t>iOS and Android devices with internet connection and access to respective app stores</t>
-  </si>
-  <si>
-    <t>1. Navigate through physics sections                                                     2. Check all chapters                                                                                   
-3. Verify same content has every chapter</t>
   </si>
   <si>
     <t>1. Open Apple App Store on iOS device
@@ -626,6 +574,60 @@
   </si>
   <si>
     <t>App demonstrates good cross-platform availability and compatibility. Installation process is smooth on both iOS and Android platforms. App icon maintains consistent branding across different operating systems.</t>
+  </si>
+  <si>
+    <t>Test hamburger menu options, screen layout, text consistency across platforms</t>
+  </si>
+  <si>
+    <t>1. Open app on Android device
+2. Access hamburger menu
+3. Note all available options
+4. Open app on iPhone
+5. Access hamburger menu
+6. Compare options between platforms
+7. Check all text and screen layout</t>
+  </si>
+  <si>
+    <t>Hamburger menu should have identical options on both Android and iPhone and the all text consistency, screen layout should same on both.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamburger menu has same options for Android and iPhone but 2 options are missing for iPhone while available for Android. The text heading not showing and also the text alignment is not same on iphone but the alignment right on android. </t>
+  </si>
+  <si>
+    <t>Platform inconsistency:  iPhone missing 2 menu options, the text alignment improper. Cross-platform inconsistency affecting user experience.</t>
+  </si>
+  <si>
+    <t>Text hierarchy implementation is inconsistent across different sections, highlighting issue and some pages are blank</t>
+  </si>
+  <si>
+    <t>Example content should load within 2-3 seconds</t>
+  </si>
+  <si>
+    <t>1. Navigate to any subject section
+2. Observe heading styles
+3. Check subheading formatting
+4. Verify body text formatting and text alignment
+5. Verify consistency across sections                                                                 6. Verify every page has text 
+7. Check Questions highlighting</t>
+  </si>
+  <si>
+    <t>Clear text hierarchy with consistent heading styles, text alignment, proper typography levels</t>
+  </si>
+  <si>
+    <t>Heading styles and text hierarchy and alignment need standardization. Affects content readability and user experiences.</t>
+  </si>
+  <si>
+    <t>Verify every chapter and subject has same content</t>
+  </si>
+  <si>
+    <t>Every chapter and subject should same content or section</t>
+  </si>
+  <si>
+    <t>In Physics, there are some chapters have short questions, while others do not and MCQ are not available</t>
+  </si>
+  <si>
+    <t>1. Navigate through physics sections                                                     2. Check all chapters                                                                                   
+3. Verify same content has every chapter and subject</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8F562D-2E0B-4C92-B0E5-74769AE8C4D5}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1096,28 +1098,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1125,28 +1127,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1154,28 +1156,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,28 +1185,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -1212,28 +1214,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1241,28 +1243,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1270,28 +1272,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1299,28 +1301,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,28 +1330,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1357,28 +1359,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,28 +1388,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1415,28 +1417,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1444,28 +1446,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1473,28 +1475,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1502,7 +1504,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>10</v>
@@ -1531,7 +1533,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>16</v>
@@ -1546,7 +1548,7 @@
         <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>9</v>
@@ -1560,7 +1562,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>10</v>
@@ -1569,48 +1571,48 @@
         <v>21</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>22</v>
+        <v>150</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1618,28 +1620,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1647,28 +1649,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,28 +1678,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,28 +1707,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1734,28 +1736,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1763,28 +1765,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,28 +1794,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>